<commit_message>
updates to PIBQ and Roulotte
</commit_message>
<xml_diff>
--- a/gayShawl/PIBQmath.xlsx
+++ b/gayShawl/PIBQmath.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shanel Wu\Box Sync\Knitting\Patterns\gayShawl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shanel Wu\Box Sync\Knitting\SWknittingdesigns\gayShawl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7ED6B58-CB5E-4AB5-BD13-EAB8C76C9C76}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7662CB8-C37A-405D-B677-8BC8C5EDE419}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A569633D-4907-4BAE-83CC-B4A4E0B25501}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{A569633D-4907-4BAE-83CC-B4A4E0B25501}"/>
   </bookViews>
   <sheets>
     <sheet name="st counts &amp; ridges" sheetId="1" r:id="rId1"/>
@@ -233,9 +233,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -248,8 +247,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1534,8 +1534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C1EBF6A-002B-496C-BEAA-0C8C73A98F2B}">
   <dimension ref="A2:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1545,7 +1545,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -1568,7 +1568,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="8"/>
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1589,7 +1589,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1615,7 +1615,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
@@ -1643,7 +1643,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -1669,7 +1669,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -1694,28 +1694,28 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="11" t="s">
+    <row r="8" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="6">
         <f>_xlfn.FLOOR.MATH((C5-3)/3)+1</f>
         <v>10</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="6">
         <f t="shared" ref="D8:G8" si="4">_xlfn.FLOOR.MATH((D5-3)/3)+1</f>
         <v>10</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="6">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="6">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="6">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
@@ -1749,7 +1749,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B10" t="s">
@@ -1772,7 +1772,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="10"/>
       <c r="B11" t="s">
         <v>12</v>
       </c>
@@ -1798,7 +1798,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+      <c r="A12" s="10"/>
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -1824,7 +1824,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+      <c r="A13" s="10"/>
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -1850,7 +1850,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
+      <c r="A14" s="10"/>
       <c r="B14" t="s">
         <v>14</v>
       </c>
@@ -1875,34 +1875,34 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10" t="s">
+    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="5">
         <f>C8</f>
         <v>10</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="5">
         <f t="shared" ref="D15:G15" si="8">D8</f>
         <v>10</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="5">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="5">
         <f t="shared" si="8"/>
         <v>11</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="5">
         <f t="shared" si="8"/>
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="3" t="s">
         <v>16</v>
       </c>
@@ -1953,7 +1953,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B18" t="s">
@@ -1980,28 +1980,28 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="11" t="s">
+    <row r="19" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="6">
         <f>_xlfn.FLOOR.MATH((C18-3)/3)+1</f>
         <v>13</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="6">
         <f t="shared" ref="D19:G19" si="11">_xlfn.FLOOR.MATH((D18-3)/3)+1</f>
         <v>13</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="6">
         <f t="shared" si="11"/>
         <v>14</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="6">
         <f t="shared" si="11"/>
         <v>14</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="6">
         <f t="shared" si="11"/>
         <v>15</v>
       </c>
@@ -2032,7 +2032,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
@@ -2059,34 +2059,34 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="10" t="s">
+    <row r="22" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="5">
         <f>C19</f>
         <v>13</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="5">
         <f t="shared" ref="D22:G22" si="14">D19</f>
         <v>13</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="5">
         <f t="shared" si="14"/>
         <v>14</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="5">
         <f t="shared" si="14"/>
         <v>14</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="5">
         <f t="shared" si="14"/>
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="3" t="s">
         <v>16</v>
       </c>
@@ -2137,7 +2137,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
@@ -2164,28 +2164,28 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="11" t="s">
+    <row r="26" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="6">
         <f>_xlfn.FLOOR.MATH((C25-3)/3)+1</f>
         <v>18</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="6">
         <f t="shared" ref="D26" si="18">_xlfn.FLOOR.MATH((D25-3)/3)+1</f>
         <v>18</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="6">
         <f t="shared" ref="E26" si="19">_xlfn.FLOOR.MATH((E25-3)/3)+1</f>
         <v>19</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="6">
         <f t="shared" ref="F26" si="20">_xlfn.FLOOR.MATH((F25-3)/3)+1</f>
         <v>19</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="6">
         <f t="shared" ref="G26" si="21">_xlfn.FLOOR.MATH((G25-3)/3)+1</f>
         <v>20</v>
       </c>
@@ -2216,7 +2216,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B28" t="s">
@@ -2243,34 +2243,34 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="10" t="s">
+    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="B29" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="5">
         <f>C26</f>
         <v>18</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="5">
         <f t="shared" ref="D29:G29" si="30">D26</f>
         <v>18</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="5">
         <f t="shared" si="30"/>
         <v>19</v>
       </c>
-      <c r="F29" s="10">
+      <c r="F29" s="5">
         <f t="shared" si="30"/>
         <v>19</v>
       </c>
-      <c r="G29" s="10">
+      <c r="G29" s="5">
         <f t="shared" si="30"/>
         <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="3" t="s">
         <v>16</v>
       </c>
@@ -2321,7 +2321,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B32" t="s">
@@ -2348,28 +2348,28 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="11" t="s">
+    <row r="33" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="6">
         <f>_xlfn.FLOOR.MATH((C32-3)/3)+1</f>
         <v>24</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="6">
         <f t="shared" ref="D33" si="40">_xlfn.FLOOR.MATH((D32-3)/3)+1</f>
         <v>24</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E33" s="6">
         <f t="shared" ref="E33" si="41">_xlfn.FLOOR.MATH((E32-3)/3)+1</f>
         <v>25</v>
       </c>
-      <c r="F33" s="11">
+      <c r="F33" s="6">
         <f t="shared" ref="F33" si="42">_xlfn.FLOOR.MATH((F32-3)/3)+1</f>
         <v>26</v>
       </c>
-      <c r="G33" s="11">
+      <c r="G33" s="6">
         <f t="shared" ref="G33" si="43">_xlfn.FLOOR.MATH((G32-3)/3)+1</f>
         <v>27</v>
       </c>
@@ -2400,7 +2400,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B35" t="s">
@@ -2427,34 +2427,34 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="10" t="s">
+    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="B36" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="5">
         <f>C33</f>
         <v>24</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="5">
         <f t="shared" ref="D36:G36" si="52">D33</f>
         <v>24</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="5">
         <f t="shared" si="52"/>
         <v>25</v>
       </c>
-      <c r="F36" s="10">
+      <c r="F36" s="5">
         <f t="shared" si="52"/>
         <v>26</v>
       </c>
-      <c r="G36" s="10">
+      <c r="G36" s="5">
         <f t="shared" si="52"/>
         <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="3" t="s">
         <v>16</v>
       </c>
@@ -2505,7 +2505,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B39" t="s">
@@ -2532,28 +2532,28 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="11" t="s">
+    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="11">
+      <c r="C40" s="6">
         <f>_xlfn.FLOOR.MATH((C39-3)/3)+1</f>
         <v>32</v>
       </c>
-      <c r="D40" s="11">
+      <c r="D40" s="6">
         <f t="shared" ref="D40" si="62">_xlfn.FLOOR.MATH((D39-3)/3)+1</f>
         <v>33</v>
       </c>
-      <c r="E40" s="11">
+      <c r="E40" s="6">
         <f t="shared" ref="E40" si="63">_xlfn.FLOOR.MATH((E39-3)/3)+1</f>
         <v>34</v>
       </c>
-      <c r="F40" s="11">
+      <c r="F40" s="6">
         <f t="shared" ref="F40" si="64">_xlfn.FLOOR.MATH((F39-3)/3)+1</f>
         <v>35</v>
       </c>
-      <c r="G40" s="11">
+      <c r="G40" s="6">
         <f t="shared" ref="G40" si="65">_xlfn.FLOOR.MATH((G39-3)/3)+1</f>
         <v>36</v>
       </c>
@@ -2584,7 +2584,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B42" t="s">
@@ -2611,34 +2611,34 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="10" t="s">
+    <row r="43" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="B43" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="5">
         <f>C40</f>
         <v>32</v>
       </c>
-      <c r="D43" s="10">
+      <c r="D43" s="5">
         <f t="shared" ref="D43:G43" si="74">D40</f>
         <v>33</v>
       </c>
-      <c r="E43" s="10">
+      <c r="E43" s="5">
         <f t="shared" si="74"/>
         <v>34</v>
       </c>
-      <c r="F43" s="10">
+      <c r="F43" s="5">
         <f t="shared" si="74"/>
         <v>35</v>
       </c>
-      <c r="G43" s="10">
+      <c r="G43" s="5">
         <f t="shared" si="74"/>
         <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
+      <c r="A44" s="11"/>
       <c r="B44" s="3" t="s">
         <v>16</v>
       </c>
@@ -2689,7 +2689,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B46" t="s">
@@ -2716,28 +2716,28 @@
         <v>147</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="11" t="s">
+    <row r="47" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C47" s="11">
+      <c r="C47" s="6">
         <f>_xlfn.FLOOR.MATH((C46-3)/3)+1</f>
         <v>43</v>
       </c>
-      <c r="D47" s="11">
+      <c r="D47" s="6">
         <f t="shared" ref="D47" si="84">_xlfn.FLOOR.MATH((D46-3)/3)+1</f>
         <v>44</v>
       </c>
-      <c r="E47" s="11">
+      <c r="E47" s="6">
         <f t="shared" ref="E47" si="85">_xlfn.FLOOR.MATH((E46-3)/3)+1</f>
         <v>46</v>
       </c>
-      <c r="F47" s="11">
+      <c r="F47" s="6">
         <f t="shared" ref="F47" si="86">_xlfn.FLOOR.MATH((F46-3)/3)+1</f>
         <v>47</v>
       </c>
-      <c r="G47" s="11">
+      <c r="G47" s="6">
         <f t="shared" ref="G47" si="87">_xlfn.FLOOR.MATH((G46-3)/3)+1</f>
         <v>49</v>
       </c>
@@ -2768,7 +2768,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B49" t="s">
@@ -2795,34 +2795,34 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="10" t="s">
+    <row r="50" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="11"/>
+      <c r="B50" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C50" s="10">
+      <c r="C50" s="5">
         <f>C47</f>
         <v>43</v>
       </c>
-      <c r="D50" s="10">
+      <c r="D50" s="5">
         <f t="shared" ref="D50:G50" si="96">D47</f>
         <v>44</v>
       </c>
-      <c r="E50" s="10">
+      <c r="E50" s="5">
         <f t="shared" si="96"/>
         <v>46</v>
       </c>
-      <c r="F50" s="10">
+      <c r="F50" s="5">
         <f t="shared" si="96"/>
         <v>47</v>
       </c>
-      <c r="G50" s="10">
+      <c r="G50" s="5">
         <f t="shared" si="96"/>
         <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
+      <c r="A51" s="11"/>
       <c r="B51" s="3" t="s">
         <v>16</v>
       </c>
@@ -2874,12 +2874,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A10:A16"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A21:A23"/>
     <mergeCell ref="A49:A51"/>
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A32:A33"/>
@@ -2887,6 +2881,12 @@
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A42:A44"/>
     <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A21:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2896,8 +2896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4595F9F5-02B6-43E9-8A51-D5732D4C42E0}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2934,7 +2934,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <f>'st counts &amp; ridges'!E8</f>
@@ -2959,7 +2959,7 @@
       </c>
       <c r="C3">
         <f>C2*(D3*E3)/(D2*E2)</f>
-        <v>3.6936170212765957</v>
+        <v>1.8468085106382979</v>
       </c>
       <c r="D3">
         <f>'st counts &amp; ridges'!E19</f>
@@ -2984,7 +2984,7 @@
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C7" si="1">C3*(D4*E4)/(D3*E3)</f>
-        <v>6.6297872340425537</v>
+        <v>3.3148936170212768</v>
       </c>
       <c r="D4">
         <f>'st counts &amp; ridges'!E26</f>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>11.48936170212766</v>
+        <v>5.7446808510638299</v>
       </c>
       <c r="D5">
         <f>'st counts &amp; ridges'!E33</f>
@@ -3020,7 +3020,7 @@
         <v>108</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f>E5/D5</f>
         <v>4.32</v>
       </c>
     </row>
@@ -3034,7 +3034,7 @@
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>20.689361702127659</v>
+        <v>10.34468085106383</v>
       </c>
       <c r="D6">
         <f>'st counts &amp; ridges'!E40</f>
@@ -3059,7 +3059,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>37.191489361702125</v>
+        <v>18.595744680851062</v>
       </c>
       <c r="D7">
         <f>'st counts &amp; ridges'!E47</f>
@@ -3089,31 +3089,31 @@
       </c>
       <c r="H9">
         <f>SUM(C2:C10)</f>
-        <v>81.693617021276594</v>
+        <v>40.846808510638297</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12">
-        <f>B3/B2*B3</f>
-        <v>3.4107016749660479</v>
+        <f>B3/B2</f>
+        <v>1.8468085106382979</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13">
-        <f>B4/B3*B4</f>
-        <v>5.9500049024414166</v>
+        <f>B4/B3</f>
+        <v>1.7949308755760369</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14">
-        <f>B5/B4*B5</f>
-        <v>9.9554802938846851</v>
+        <f>B5/B4</f>
+        <v>1.7329910141206675</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D15">
-        <f>B6/B5*B6</f>
-        <v>18.628088258471237</v>
+        <f>B6/B5</f>
+        <v>1.8007407407407408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>